<commit_message>
- MMA and more
</commit_message>
<xml_diff>
--- a/updates.xlsx
+++ b/updates.xlsx
@@ -736,7 +736,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection sqref="A1:L24"/>
+      <selection activeCell="L1" sqref="A1:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,11 +957,11 @@
       <c r="H6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="21" t="s">
+      <c r="I6" s="21" t="s">
         <v>13</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>15</v>
       </c>
       <c r="K6" s="21" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Update NVH, CSE and IAAM
</commit_message>
<xml_diff>
--- a/updates.xlsx
+++ b/updates.xlsx
@@ -141,9 +141,6 @@
     <t>- planned support</t>
   </si>
   <si>
-    <t>momentariymodder.xyz</t>
-  </si>
-  <si>
     <t>Storage Crate</t>
   </si>
   <si>
@@ -195,7 +192,10 @@
     <t>It's All About Money Reload</t>
   </si>
   <si>
-    <t>26.09.2024, 16:30 (MSK)</t>
+    <t>14.11.2024, 05:00 (MSK)</t>
+  </si>
+  <si>
+    <t>momentariymodder.netlify.app</t>
   </si>
 </sst>
 </file>
@@ -558,6 +558,18 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -567,19 +579,7 @@
     <xf numFmtId="49" fontId="8" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -865,7 +865,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection sqref="A1:O29"/>
+      <selection activeCell="O29" sqref="A1:O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,9 +878,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51"/>
-      <c r="B1" s="51"/>
-      <c r="C1" s="54" t="s">
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="57" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="53" t="s">
@@ -909,19 +909,19 @@
       </c>
       <c r="L1" s="53"/>
       <c r="M1" s="53" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N1" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="O1" s="57" t="s">
-        <v>54</v>
+        <v>49</v>
+      </c>
+      <c r="O1" s="52" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="54"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="57"/>
       <c r="D2" s="53"/>
       <c r="E2" s="53"/>
       <c r="F2" s="53"/>
@@ -936,29 +936,29 @@
       <c r="O2" s="53"/>
     </row>
     <row r="3" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
       <c r="K3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
+      <c r="M3" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
     </row>
     <row r="4" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
@@ -1022,18 +1022,18 @@
       <c r="J5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="55"/>
+      <c r="K5" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="50"/>
       <c r="M5" s="43" t="s">
         <v>10</v>
       </c>
       <c r="N5" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="39" t="s">
-        <v>11</v>
+      <c r="O5" s="42" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1092,18 +1092,18 @@
       <c r="J7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="55"/>
+      <c r="K7" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="50"/>
       <c r="M7" s="43" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="39" t="s">
-        <v>11</v>
+      <c r="O7" s="42" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1111,7 +1111,7 @@
         <v>28</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="49"/>
       <c r="D8" s="49"/>
@@ -1129,8 +1129,8 @@
       <c r="N8" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="39" t="s">
-        <v>11</v>
+      <c r="O8" s="42" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1138,7 +1138,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
@@ -1175,10 +1175,10 @@
         <v>10</v>
       </c>
       <c r="J10" s="28"/>
-      <c r="K10" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="L10" s="55"/>
+      <c r="K10" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="50"/>
       <c r="M10" s="46" t="s">
         <v>10</v>
       </c>
@@ -1208,8 +1208,8 @@
       <c r="J11" s="49"/>
       <c r="K11" s="49"/>
       <c r="L11" s="49"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
       <c r="O11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1233,8 +1233,8 @@
       <c r="J12" s="49"/>
       <c r="K12" s="49"/>
       <c r="L12" s="49"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
       <c r="O12" s="49"/>
     </row>
     <row r="13" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1256,8 +1256,8 @@
       <c r="J13" s="49"/>
       <c r="K13" s="49"/>
       <c r="L13" s="49"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="50"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="54"/>
       <c r="O13" s="49"/>
     </row>
     <row r="14" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1283,8 +1283,8 @@
       <c r="J14" s="49"/>
       <c r="K14" s="49"/>
       <c r="L14" s="49"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
       <c r="O14" s="49"/>
     </row>
     <row r="15" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1314,8 +1314,8 @@
       <c r="J15" s="49"/>
       <c r="K15" s="49"/>
       <c r="L15" s="49"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
       <c r="O15" s="49"/>
     </row>
     <row r="16" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1335,12 +1335,12 @@
       <c r="H16" s="49"/>
       <c r="I16" s="49"/>
       <c r="J16" s="49"/>
-      <c r="K16" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="55"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="50"/>
+      <c r="K16" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="50"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
       <c r="O16" s="44"/>
     </row>
     <row r="17" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1362,8 +1362,8 @@
       <c r="J17" s="49"/>
       <c r="K17" s="49"/>
       <c r="L17" s="49"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="50"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54"/>
       <c r="O17" s="49"/>
     </row>
     <row r="18" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1371,7 +1371,7 @@
         <v>28</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="36"/>
       <c r="D18" s="36"/>
@@ -1442,7 +1442,7 @@
         <v>27</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="11"/>
@@ -1490,7 +1490,7 @@
       <c r="F23" s="11"/>
       <c r="G23" s="28"/>
       <c r="H23" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="11"/>
@@ -1529,7 +1529,7 @@
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
@@ -1552,12 +1552,12 @@
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="22" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
@@ -1577,12 +1577,12 @@
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
@@ -1598,12 +1598,12 @@
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
       <c r="J28" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
@@ -1630,13 +1630,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="N11:N17"/>
-    <mergeCell ref="M11:M17"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="M1:M2"/>
@@ -1649,6 +1642,13 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="K1:L2"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="N11:N17"/>
+    <mergeCell ref="M11:M17"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="K10:L10"/>
   </mergeCells>

</xml_diff>

<commit_message>
CMD 3.10.0 & 6.0.0
</commit_message>
<xml_diff>
--- a/updates.xlsx
+++ b/updates.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
   <si>
     <t>1.12.2</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Created Spawn Eggs</t>
   </si>
   <si>
-    <t>PerodiumCraft</t>
-  </si>
-  <si>
     <t>SpongeBob Squarepants Reload</t>
   </si>
   <si>
@@ -183,26 +180,38 @@
     <t>LF - Forge</t>
   </si>
   <si>
-    <t>- no information, or no plans, or cancelled</t>
-  </si>
-  <si>
     <t>1.21.1</t>
   </si>
   <si>
     <t>It's All About Money Reload</t>
   </si>
   <si>
-    <t>14.11.2024, 05:00 (MSK)</t>
-  </si>
-  <si>
     <t>momentariymodder.netlify.app</t>
+  </si>
+  <si>
+    <t>Canceled</t>
+  </si>
+  <si>
+    <t>- no information, or no plans</t>
+  </si>
+  <si>
+    <t>- support is cancelled</t>
+  </si>
+  <si>
+    <t>28.11.2024, 22:00 (MSK)</t>
+  </si>
+  <si>
+    <t>PerodiumCraft: Old</t>
+  </si>
+  <si>
+    <t>PerodiumCraft: The New Generation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,14 +307,6 @@
     </font>
     <font>
       <b/>
-      <sz val="22"/>
-      <color theme="0"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Segoe UI"/>
@@ -320,8 +321,24 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,6 +417,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -413,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -477,9 +506,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -487,9 +513,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -510,28 +533,19 @@
     <xf numFmtId="49" fontId="6" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -549,25 +563,13 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -579,7 +581,31 @@
     <xf numFmtId="49" fontId="8" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -588,6 +614,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCC00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -862,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="O29" sqref="A1:O29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,98 +909,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="57" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" s="53" t="s">
+      <c r="L1" s="48"/>
+      <c r="M1" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+    </row>
+    <row r="3" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="51" t="s">
         <v>49</v>
-      </c>
-      <c r="O1" s="52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-    </row>
-    <row r="3" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="51" t="s">
-        <v>50</v>
       </c>
       <c r="N3" s="51"/>
       <c r="O3" s="51"/>
     </row>
     <row r="4" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="32" t="s">
+      <c r="A4" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="17" t="s">
         <v>10</v>
       </c>
@@ -985,34 +1016,32 @@
       <c r="J4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="O4" s="42" t="s">
+      <c r="K4" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="50"/>
+      <c r="M4" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="32" t="s">
+      <c r="A5" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
       <c r="H5" s="17" t="s">
         <v>10</v>
       </c>
@@ -1026,28 +1055,28 @@
         <v>10</v>
       </c>
       <c r="L5" s="50"/>
-      <c r="M5" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="N5" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="O5" s="42" t="s">
+      <c r="M5" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="32" t="s">
+      <c r="A6" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="17" t="s">
         <v>10</v>
       </c>
@@ -1057,35 +1086,35 @@
       <c r="J6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="42" t="s">
+      <c r="K6" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="N6" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="O6" s="39" t="s">
-        <v>11</v>
+      <c r="L6" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="37" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
       <c r="I7" s="17" t="s">
         <v>10</v>
       </c>
@@ -1096,319 +1125,331 @@
         <v>10</v>
       </c>
       <c r="L7" s="50"/>
-      <c r="M7" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="N7" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="O7" s="42" t="s">
+      <c r="M7" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>28</v>
+      <c r="A8" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="B8" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="O8" s="42" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="36"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="39" t="s">
+      <c r="L9" s="33"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="O9" s="55" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="26"/>
+      <c r="K10" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="50"/>
+      <c r="M10" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="43"/>
+    </row>
+    <row r="12" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="43"/>
+    </row>
+    <row r="13" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="43"/>
+    </row>
+    <row r="14" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="45"/>
+    </row>
+    <row r="15" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="45"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="43"/>
+    </row>
+    <row r="16" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="43"/>
+      <c r="D16" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="43"/>
+    </row>
+    <row r="17" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B17" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="28"/>
-      <c r="K10" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="L10" s="50"/>
-      <c r="M10" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="N10" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="O10" s="42" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="54"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="49"/>
-    </row>
-    <row r="12" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="49"/>
-    </row>
-    <row r="13" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="14" t="s">
+      <c r="C17" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="50"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+    </row>
+    <row r="18" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="26" t="s">
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="43"/>
+    </row>
+    <row r="19" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="54"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="49"/>
-    </row>
-    <row r="14" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="49"/>
-    </row>
-    <row r="15" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="49"/>
-    </row>
-    <row r="16" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="50"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="44"/>
-    </row>
-    <row r="17" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="49"/>
-    </row>
-    <row r="18" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="36"/>
-      <c r="K18" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18" s="36"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-    </row>
-    <row r="19" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
+      <c r="B19" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="33"/>
+      <c r="K19" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19" s="33"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
     </row>
     <row r="20" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
@@ -1430,21 +1471,21 @@
     <row r="21" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="37" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="26" t="s">
-        <v>27</v>
+      <c r="G21" s="25" t="s">
+        <v>26</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="I21" s="10"/>
+        <v>41</v>
+      </c>
+      <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
@@ -1455,61 +1496,65 @@
     <row r="22" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="23" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="27" t="s">
+      <c r="G22" s="55" t="s">
         <v>11</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
       <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
-      <c r="G23" s="28"/>
+      <c r="G23" s="45"/>
       <c r="H23" s="20" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
       <c r="O23" s="11"/>
     </row>
     <row r="24" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="21"/>
+      <c r="C24" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>56</v>
+      </c>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
+      <c r="I24" s="10"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
@@ -1518,47 +1563,39 @@
       <c r="O24" s="11"/>
     </row>
     <row r="25" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-    </row>
-    <row r="26" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+    </row>
+    <row r="26" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>30</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
-      <c r="G26" s="33" t="s">
-        <v>45</v>
+      <c r="G26" s="28" t="s">
+        <v>50</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
-      <c r="J26" s="22" t="s">
-        <v>56</v>
-      </c>
+      <c r="J26" s="10"/>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
@@ -1572,17 +1609,17 @@
         <v>29</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="30" t="s">
-        <v>39</v>
+      <c r="G27" s="31" t="s">
+        <v>44</v>
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="22" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
@@ -1593,17 +1630,21 @@
     <row r="28" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
+      <c r="C28" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>32</v>
+      </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
-      <c r="G28" s="30" t="s">
-        <v>46</v>
+      <c r="G28" s="28" t="s">
+        <v>38</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
       <c r="J28" s="22" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
@@ -1611,25 +1652,54 @@
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
     </row>
-    <row r="29" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="G29" s="28" t="s">
+        <v>45</v>
+      </c>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
+      <c r="J29" s="22" t="s">
+        <v>57</v>
+      </c>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
     </row>
+    <row r="30" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="20">
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K4:L4"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="M1:M2"/>
@@ -1642,15 +1712,6 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="K1:L2"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="N11:N17"/>
-    <mergeCell ref="M11:M17"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1682,7 +1743,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>11</v>

</xml_diff>